<commit_message>
added new columns to spreadsheet
</commit_message>
<xml_diff>
--- a/wide format analysis.xlsx
+++ b/wide format analysis.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27417"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="223" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41087BCB-BE26-4504-8EF7-15B16DD8CECC}"/>
+  <xr:revisionPtr revIDLastSave="241" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34882290-6755-4D01-BED6-E7A954CBBB34}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="281">
   <si>
     <t xml:space="preserve">Column Names                                                                                </t>
   </si>
@@ -75,615 +75,618 @@
     <t>income                                         numeric</t>
   </si>
   <si>
+    <t>continuous 32000 - 120000</t>
+  </si>
+  <si>
+    <t>tenure                                         numeric</t>
+  </si>
+  <si>
+    <t>1 to 600+</t>
+  </si>
+  <si>
+    <t>tot_off_rec                                    numeric</t>
+  </si>
+  <si>
+    <t>0 to 6 Count</t>
+  </si>
+  <si>
+    <t>tot_off_view                                   numeric</t>
+  </si>
+  <si>
+    <t>tot_off_comp                                   numeric</t>
+  </si>
+  <si>
+    <t>tot_reward                                     numeric</t>
+  </si>
+  <si>
+    <t>0 to 50</t>
+  </si>
+  <si>
+    <t>tot_trans                                      numeric</t>
+  </si>
+  <si>
+    <t>Count 0-36</t>
+  </si>
+  <si>
+    <t>tot_amount                                     numeric</t>
+  </si>
+  <si>
+    <t>Continuous  0-1608</t>
+  </si>
+  <si>
+    <t>ave_amount                                     numeric</t>
+  </si>
+  <si>
+    <t>Continuous 0-136</t>
+  </si>
+  <si>
+    <t>max_amount                                     numeric</t>
+  </si>
+  <si>
+    <t>Continuous 0-1062</t>
+  </si>
+  <si>
+    <t>off_rec_offer10                                numeric</t>
+  </si>
+  <si>
+    <t>Count 0 to 4 - 5 nas</t>
+  </si>
+  <si>
+    <t>off_rec_offer3                                 numeric</t>
+  </si>
+  <si>
+    <t>off_rec_offer7                                 numeric</t>
+  </si>
+  <si>
+    <t>off_rec_offer8                                 numeric</t>
+  </si>
+  <si>
+    <t>off_rec_offer9                                 numeric</t>
+  </si>
+  <si>
+    <t>off_rec_offer4                                 numeric</t>
+  </si>
+  <si>
+    <t>off_rec_offer5                                 numeric</t>
+  </si>
+  <si>
+    <t>off_rec_offer6                                 numeric</t>
+  </si>
+  <si>
+    <t>off_rec_offer1                                 numeric</t>
+  </si>
+  <si>
+    <t>off_rec_offer2                                 numeric</t>
+  </si>
+  <si>
+    <t>off_view_offer10                               numeric</t>
+  </si>
+  <si>
+    <t>off_view_offer3                                numeric</t>
+  </si>
+  <si>
+    <t>off_view_offer7                                numeric</t>
+  </si>
+  <si>
+    <t>off_view_offer8                                numeric</t>
+  </si>
+  <si>
+    <t>off_view_offer9                                numeric</t>
+  </si>
+  <si>
+    <t>off_view_offer4                                numeric</t>
+  </si>
+  <si>
+    <t>off_view_offer5                                numeric</t>
+  </si>
+  <si>
+    <t>off_view_offer6                                numeric</t>
+  </si>
+  <si>
+    <t>off_view_offer1                                numeric</t>
+  </si>
+  <si>
+    <t>off_view_offer2                                numeric</t>
+  </si>
+  <si>
+    <t>off_comp_offer10                               numeric</t>
+  </si>
+  <si>
+    <t>off_comp_offer3                                numeric</t>
+  </si>
+  <si>
+    <t>off_comp_offer7                                numeric</t>
+  </si>
+  <si>
+    <t>off_comp_offer8                                numeric</t>
+  </si>
+  <si>
+    <t>off_comp_offer9                                numeric</t>
+  </si>
+  <si>
+    <t>off_comp_offer4                                numeric</t>
+  </si>
+  <si>
+    <t>off_comp_offer5                                numeric</t>
+  </si>
+  <si>
+    <t>off_comp_offer6                                numeric</t>
+  </si>
+  <si>
+    <t>off_comp_offer1                                numeric</t>
+  </si>
+  <si>
+    <t>off_comp_offer2                                numeric</t>
+  </si>
+  <si>
+    <t>tot_reward_offer10                             numeric</t>
+  </si>
+  <si>
+    <t>Sum of reward 0 to 8 -5 na</t>
+  </si>
+  <si>
+    <t>tot_reward_offer3                              numeric</t>
+  </si>
+  <si>
+    <t>Sum of reward 0   5 na</t>
+  </si>
+  <si>
+    <t>tot_reward_offer7                              numeric</t>
+  </si>
+  <si>
+    <t>Sum of reward 0 to 10</t>
+  </si>
+  <si>
+    <t>tot_reward_offer8                              numeric</t>
+  </si>
+  <si>
+    <t>tot_reward_offer9                              numeric</t>
+  </si>
+  <si>
+    <t>tot_reward_offer4                              numeric</t>
+  </si>
+  <si>
+    <t>tot_reward_offer5                              numeric</t>
+  </si>
+  <si>
+    <t>tot_reward_offer6                              numeric</t>
+  </si>
+  <si>
+    <t>tot_reward_offer1                              numeric</t>
+  </si>
+  <si>
+    <t>tot_reward_offer2                              numeric</t>
+  </si>
+  <si>
+    <t>trans_offer10                                  numeric</t>
+  </si>
+  <si>
+    <t>Count transactions in offer period roughly 0-40. 5 na</t>
+  </si>
+  <si>
+    <t>trans_offer3                                   numeric</t>
+  </si>
+  <si>
+    <t>trans_offer7                                   numeric</t>
+  </si>
+  <si>
+    <t>trans_offer8                                   numeric</t>
+  </si>
+  <si>
+    <t>trans_offer9                                   numeric</t>
+  </si>
+  <si>
+    <t>trans_offer4                                   numeric</t>
+  </si>
+  <si>
+    <t>trans_offer5                                   numeric</t>
+  </si>
+  <si>
+    <t>trans_offer6                                   numeric</t>
+  </si>
+  <si>
+    <t>trans_offer1                                   numeric</t>
+  </si>
+  <si>
+    <t>trans_offer2                                   numeric</t>
+  </si>
+  <si>
+    <t>amount_offer10                                 numeric</t>
+  </si>
+  <si>
+    <t>Continuous - amount spent in offer period 5 nas</t>
+  </si>
+  <si>
+    <t>amount_offer3                                  numeric</t>
+  </si>
+  <si>
+    <t>amount_offer7                                  numeric</t>
+  </si>
+  <si>
+    <t>amount_offer8                                  numeric</t>
+  </si>
+  <si>
+    <t>amount_offer9                                  numeric</t>
+  </si>
+  <si>
+    <t>amount_offer4                                  numeric</t>
+  </si>
+  <si>
+    <t>amount_offer5                                  numeric</t>
+  </si>
+  <si>
+    <t>amount_offer6                                  numeric</t>
+  </si>
+  <si>
+    <t>amount_offer1                                  numeric</t>
+  </si>
+  <si>
+    <t>amount_offer2                                  numeric</t>
+  </si>
+  <si>
+    <t>reward_off_offer1                              numeric</t>
+  </si>
+  <si>
+    <t>1 unique value of reward value</t>
+  </si>
+  <si>
+    <t>Since all the same does it help in clusetering?</t>
+  </si>
+  <si>
+    <t>reward_off_offer2                              numeric</t>
+  </si>
+  <si>
+    <t>reward_off_offer3                              numeric</t>
+  </si>
+  <si>
+    <t>reward_off_offer4                              numeric</t>
+  </si>
+  <si>
+    <t>reward_off_offer5                              numeric</t>
+  </si>
+  <si>
+    <t>reward_off_offer6                              numeric</t>
+  </si>
+  <si>
+    <t>reward_off_offer7                              numeric</t>
+  </si>
+  <si>
+    <t>reward_off_offer8                              numeric</t>
+  </si>
+  <si>
+    <t>reward_off_offer9                              numeric</t>
+  </si>
+  <si>
+    <t>reward_off_offer10                             numeric</t>
+  </si>
+  <si>
+    <t>difficulty_offer1                              numeric</t>
+  </si>
+  <si>
+    <t>1 unique value of amount to spend to get reward</t>
+  </si>
+  <si>
+    <t>difficulty_offer2                              numeric</t>
+  </si>
+  <si>
+    <t>difficulty_offer3                              numeric</t>
+  </si>
+  <si>
+    <t>difficulty_offer4                              numeric</t>
+  </si>
+  <si>
+    <t>difficulty_offer5                              numeric</t>
+  </si>
+  <si>
+    <t>difficulty_offer6                              numeric</t>
+  </si>
+  <si>
+    <t>difficulty_offer7                              numeric</t>
+  </si>
+  <si>
+    <t>difficulty_offer8                              numeric</t>
+  </si>
+  <si>
+    <t>difficulty_offer9                              numeric</t>
+  </si>
+  <si>
+    <t>difficulty_offer10                             numeric</t>
+  </si>
+  <si>
+    <t>duration_offer1                                numeric</t>
+  </si>
+  <si>
+    <t>duration of award in hours one unique value</t>
+  </si>
+  <si>
+    <t>duration_offer2                                numeric</t>
+  </si>
+  <si>
+    <t>duration_offer3                                numeric</t>
+  </si>
+  <si>
+    <t>duration_offer4                                numeric</t>
+  </si>
+  <si>
+    <t>duration_offer5                                numeric</t>
+  </si>
+  <si>
+    <t>duration_offer6                                numeric</t>
+  </si>
+  <si>
+    <t>duration_offer7                                numeric</t>
+  </si>
+  <si>
+    <t>duration_offer8                                numeric</t>
+  </si>
+  <si>
+    <t>duration_offer9                                numeric</t>
+  </si>
+  <si>
+    <t>duration_offer10                               numeric</t>
+  </si>
+  <si>
+    <t>bogo_offer1                                    numeric</t>
+  </si>
+  <si>
+    <t>one unique value - is offer bogo</t>
+  </si>
+  <si>
+    <t>bogo_offer2                                    numeric</t>
+  </si>
+  <si>
+    <t>bogo_offer3                                    numeric</t>
+  </si>
+  <si>
+    <t>bogo_offer4                                    numeric</t>
+  </si>
+  <si>
+    <t>bogo_offer5                                    numeric</t>
+  </si>
+  <si>
+    <t>bogo_offer6                                    numeric</t>
+  </si>
+  <si>
+    <t>bogo_offer7                                    numeric</t>
+  </si>
+  <si>
+    <t>bogo_offer8                                    numeric</t>
+  </si>
+  <si>
+    <t>bogo_offer9                                    numeric</t>
+  </si>
+  <si>
+    <t>bogo_offer10                                   numeric</t>
+  </si>
+  <si>
+    <t>discount_offer1                                numeric</t>
+  </si>
+  <si>
+    <t>one unique value - is offer discount</t>
+  </si>
+  <si>
+    <t>discount_offer2                                numeric</t>
+  </si>
+  <si>
+    <t>discount_offer3                                numeric</t>
+  </si>
+  <si>
+    <t>discount_offer4                                numeric</t>
+  </si>
+  <si>
+    <t>discount_offer5                                numeric</t>
+  </si>
+  <si>
+    <t>discount_offer6                                numeric</t>
+  </si>
+  <si>
+    <t>discount_offer7                                numeric</t>
+  </si>
+  <si>
+    <t>discount_offer8                                numeric</t>
+  </si>
+  <si>
+    <t>discount_offer9                                numeric</t>
+  </si>
+  <si>
+    <t>discount_offer10                               numeric</t>
+  </si>
+  <si>
+    <t>informational_offer1                           numeric</t>
+  </si>
+  <si>
+    <t>one unique value - is offer informational</t>
+  </si>
+  <si>
+    <t>informational_offer2                           numeric</t>
+  </si>
+  <si>
+    <t>informational_offer3                           numeric</t>
+  </si>
+  <si>
+    <t>informational_offer4                           numeric</t>
+  </si>
+  <si>
+    <t>informational_offer5                           numeric</t>
+  </si>
+  <si>
+    <t>informational_offer6                           numeric</t>
+  </si>
+  <si>
+    <t>informational_offer7                           numeric</t>
+  </si>
+  <si>
+    <t>informational_offer8                           numeric</t>
+  </si>
+  <si>
+    <t>informational_offer9                           numeric</t>
+  </si>
+  <si>
+    <t>informational_offer10                          numeric</t>
+  </si>
+  <si>
+    <t>email_offer1                                   numeric</t>
+  </si>
+  <si>
+    <t>one unique value - is offer emailed</t>
+  </si>
+  <si>
+    <t>All offers are emailed - do we need? Also one unique value no variation to detect</t>
+  </si>
+  <si>
+    <t>email_offer2                                   numeric</t>
+  </si>
+  <si>
+    <t>email_offer3                                   numeric</t>
+  </si>
+  <si>
+    <t>email_offer4                                   numeric</t>
+  </si>
+  <si>
+    <t>email_offer5                                   numeric</t>
+  </si>
+  <si>
+    <t>email_offer6                                   numeric</t>
+  </si>
+  <si>
+    <t>email_offer7                                   numeric</t>
+  </si>
+  <si>
+    <t>email_offer8                                   numeric</t>
+  </si>
+  <si>
+    <t>email_offer9                                   numeric</t>
+  </si>
+  <si>
+    <t>email_offer10                                  numeric</t>
+  </si>
+  <si>
+    <t>mobile_offer1                                  numeric</t>
+  </si>
+  <si>
+    <t>one unique value - is offer mobile</t>
+  </si>
+  <si>
+    <t>Since all the same does it help in clustering?</t>
+  </si>
+  <si>
+    <t>mobile_offer2                                  numeric</t>
+  </si>
+  <si>
+    <t>mobile_offer3                                  numeric</t>
+  </si>
+  <si>
+    <t>mobile_offer4                                  numeric</t>
+  </si>
+  <si>
+    <t>mobile_offer5                                  numeric</t>
+  </si>
+  <si>
+    <t>mobile_offer6                                  numeric</t>
+  </si>
+  <si>
+    <t>mobile_offer7                                  numeric</t>
+  </si>
+  <si>
+    <t>mobile_offer8                                  numeric</t>
+  </si>
+  <si>
+    <t>mobile_offer9                                  numeric</t>
+  </si>
+  <si>
+    <t>mobile_offer10                                 numeric</t>
+  </si>
+  <si>
+    <t>social_offer1                                  numeric</t>
+  </si>
+  <si>
+    <t>social_offer2                                  numeric</t>
+  </si>
+  <si>
+    <t>social_offer3                                  numeric</t>
+  </si>
+  <si>
+    <t>social_offer4                                  numeric</t>
+  </si>
+  <si>
+    <t>social_offer5                                  numeric</t>
+  </si>
+  <si>
+    <t>social_offer6                                  numeric</t>
+  </si>
+  <si>
+    <t>social_offer7                                  numeric</t>
+  </si>
+  <si>
+    <t>social_offer8                                  numeric</t>
+  </si>
+  <si>
+    <t>social_offer9                                  numeric</t>
+  </si>
+  <si>
+    <t>social_offer10                                 numeric</t>
+  </si>
+  <si>
+    <t>web_offer1                                     numeric</t>
+  </si>
+  <si>
+    <t>one unique value - is offer web</t>
+  </si>
+  <si>
+    <t>web_offer2                                     numeric</t>
+  </si>
+  <si>
+    <t>web_offer3                                     numeric</t>
+  </si>
+  <si>
+    <t>web_offer4                                     numeric</t>
+  </si>
+  <si>
+    <t>web_offer5                                     numeric</t>
+  </si>
+  <si>
+    <t>web_offer6                                     numeric</t>
+  </si>
+  <si>
+    <t>web_offer7                                     numeric</t>
+  </si>
+  <si>
+    <t>web_offer8                                     numeric</t>
+  </si>
+  <si>
+    <t>web_offer9                                     numeric</t>
+  </si>
+  <si>
+    <t>web_offer10                                    numeric</t>
+  </si>
+  <si>
+    <t>offer_view_rate                                numeric</t>
+  </si>
+  <si>
+    <t>continuous between zero and one 5 nas</t>
+  </si>
+  <si>
+    <t>offer_completion_rate                          numeric</t>
+  </si>
+  <si>
+    <t>view_to_completion_rate                        numeric</t>
+  </si>
+  <si>
+    <t>continuous between zero and one - infinity and nan in</t>
+  </si>
+  <si>
+    <t>average_spend_per_transaction                  numeric</t>
+  </si>
+  <si>
+    <t>difference to ave_amount? 333 nas 0.15 to 451.47</t>
+  </si>
+  <si>
+    <t>spend_per_day                                  numeric</t>
+  </si>
+  <si>
     <t>continuous</t>
   </si>
   <si>
-    <t>tenure                                         numeric</t>
-  </si>
-  <si>
-    <t>1 to 600+</t>
-  </si>
-  <si>
-    <t>tot_off_rec                                    numeric</t>
-  </si>
-  <si>
-    <t>0 to 6 Count</t>
-  </si>
-  <si>
-    <t>tot_off_view                                   numeric</t>
-  </si>
-  <si>
-    <t>tot_off_comp                                   numeric</t>
-  </si>
-  <si>
-    <t>tot_reward                                     numeric</t>
-  </si>
-  <si>
-    <t>0 to 50</t>
-  </si>
-  <si>
-    <t>tot_trans                                      numeric</t>
-  </si>
-  <si>
-    <t>Count 0-36</t>
-  </si>
-  <si>
-    <t>tot_amount                                     numeric</t>
-  </si>
-  <si>
-    <t>Continuous  0-1608</t>
-  </si>
-  <si>
-    <t>ave_amount                                     numeric</t>
-  </si>
-  <si>
-    <t>Continuous 0-136</t>
-  </si>
-  <si>
-    <t>max_amount                                     numeric</t>
-  </si>
-  <si>
-    <t>Continuous 0-1062</t>
-  </si>
-  <si>
-    <t>off_rec_offer10                                numeric</t>
-  </si>
-  <si>
-    <t>Count 0 to 4 - 5 nas</t>
-  </si>
-  <si>
-    <t>off_rec_offer3                                 numeric</t>
-  </si>
-  <si>
-    <t>off_rec_offer7                                 numeric</t>
-  </si>
-  <si>
-    <t>off_rec_offer8                                 numeric</t>
-  </si>
-  <si>
-    <t>off_rec_offer9                                 numeric</t>
-  </si>
-  <si>
-    <t>off_rec_offer4                                 numeric</t>
-  </si>
-  <si>
-    <t>off_rec_offer5                                 numeric</t>
-  </si>
-  <si>
-    <t>off_rec_offer6                                 numeric</t>
-  </si>
-  <si>
-    <t>off_rec_offer1                                 numeric</t>
-  </si>
-  <si>
-    <t>off_rec_offer2                                 numeric</t>
-  </si>
-  <si>
-    <t>off_view_offer10                               numeric</t>
-  </si>
-  <si>
-    <t>off_view_offer3                                numeric</t>
-  </si>
-  <si>
-    <t>off_view_offer7                                numeric</t>
-  </si>
-  <si>
-    <t>off_view_offer8                                numeric</t>
-  </si>
-  <si>
-    <t>off_view_offer9                                numeric</t>
-  </si>
-  <si>
-    <t>off_view_offer4                                numeric</t>
-  </si>
-  <si>
-    <t>off_view_offer5                                numeric</t>
-  </si>
-  <si>
-    <t>off_view_offer6                                numeric</t>
-  </si>
-  <si>
-    <t>off_view_offer1                                numeric</t>
-  </si>
-  <si>
-    <t>off_view_offer2                                numeric</t>
-  </si>
-  <si>
-    <t>off_comp_offer10                               numeric</t>
-  </si>
-  <si>
-    <t>off_comp_offer3                                numeric</t>
-  </si>
-  <si>
-    <t>off_comp_offer7                                numeric</t>
-  </si>
-  <si>
-    <t>off_comp_offer8                                numeric</t>
-  </si>
-  <si>
-    <t>off_comp_offer9                                numeric</t>
-  </si>
-  <si>
-    <t>off_comp_offer4                                numeric</t>
-  </si>
-  <si>
-    <t>off_comp_offer5                                numeric</t>
-  </si>
-  <si>
-    <t>off_comp_offer6                                numeric</t>
-  </si>
-  <si>
-    <t>off_comp_offer1                                numeric</t>
-  </si>
-  <si>
-    <t>off_comp_offer2                                numeric</t>
-  </si>
-  <si>
-    <t>tot_reward_offer10                             numeric</t>
-  </si>
-  <si>
-    <t>Sum of reward 0 to 8 -5 na</t>
-  </si>
-  <si>
-    <t>tot_reward_offer3                              numeric</t>
-  </si>
-  <si>
-    <t>Sum of reward 0 5 na</t>
-  </si>
-  <si>
-    <t>tot_reward_offer7                              numeric</t>
-  </si>
-  <si>
-    <t>Sum of reward 0 to 10</t>
-  </si>
-  <si>
-    <t>tot_reward_offer8                              numeric</t>
-  </si>
-  <si>
-    <t>tot_reward_offer9                              numeric</t>
-  </si>
-  <si>
-    <t>tot_reward_offer4                              numeric</t>
-  </si>
-  <si>
-    <t>tot_reward_offer5                              numeric</t>
-  </si>
-  <si>
-    <t>tot_reward_offer6                              numeric</t>
-  </si>
-  <si>
-    <t>tot_reward_offer1                              numeric</t>
-  </si>
-  <si>
-    <t>tot_reward_offer2                              numeric</t>
-  </si>
-  <si>
-    <t>trans_offer10                                  numeric</t>
-  </si>
-  <si>
-    <t>Count transactions in offer period roughly 0-40. 5 na</t>
-  </si>
-  <si>
-    <t>trans_offer3                                   numeric</t>
-  </si>
-  <si>
-    <t>trans_offer7                                   numeric</t>
-  </si>
-  <si>
-    <t>trans_offer8                                   numeric</t>
-  </si>
-  <si>
-    <t>trans_offer9                                   numeric</t>
-  </si>
-  <si>
-    <t>trans_offer4                                   numeric</t>
-  </si>
-  <si>
-    <t>trans_offer5                                   numeric</t>
-  </si>
-  <si>
-    <t>trans_offer6                                   numeric</t>
-  </si>
-  <si>
-    <t>trans_offer1                                   numeric</t>
-  </si>
-  <si>
-    <t>trans_offer2                                   numeric</t>
-  </si>
-  <si>
-    <t>amount_offer10                                 numeric</t>
-  </si>
-  <si>
-    <t>Continuous - amount spent in offer period 5 nas</t>
-  </si>
-  <si>
-    <t>amount_offer3                                  numeric</t>
-  </si>
-  <si>
-    <t>amount_offer7                                  numeric</t>
-  </si>
-  <si>
-    <t>amount_offer8                                  numeric</t>
-  </si>
-  <si>
-    <t>amount_offer9                                  numeric</t>
-  </si>
-  <si>
-    <t>amount_offer4                                  numeric</t>
-  </si>
-  <si>
-    <t>amount_offer5                                  numeric</t>
-  </si>
-  <si>
-    <t>amount_offer6                                  numeric</t>
-  </si>
-  <si>
-    <t>amount_offer1                                  numeric</t>
-  </si>
-  <si>
-    <t>amount_offer2                                  numeric</t>
-  </si>
-  <si>
-    <t>reward_off_offer1                              numeric</t>
-  </si>
-  <si>
-    <t>1 unique value of reward value</t>
-  </si>
-  <si>
-    <t>Since all the same does it help in clusetering?</t>
-  </si>
-  <si>
-    <t>reward_off_offer2                              numeric</t>
-  </si>
-  <si>
-    <t>reward_off_offer3                              numeric</t>
-  </si>
-  <si>
-    <t>reward_off_offer4                              numeric</t>
-  </si>
-  <si>
-    <t>reward_off_offer5                              numeric</t>
-  </si>
-  <si>
-    <t>reward_off_offer6                              numeric</t>
-  </si>
-  <si>
-    <t>reward_off_offer7                              numeric</t>
-  </si>
-  <si>
-    <t>reward_off_offer8                              numeric</t>
-  </si>
-  <si>
-    <t>reward_off_offer9                              numeric</t>
-  </si>
-  <si>
-    <t>reward_off_offer10                             numeric</t>
-  </si>
-  <si>
-    <t>difficulty_offer1                              numeric</t>
-  </si>
-  <si>
-    <t>1 unique value of amount to spend to get reward</t>
-  </si>
-  <si>
-    <t>difficulty_offer2                              numeric</t>
-  </si>
-  <si>
-    <t>difficulty_offer3                              numeric</t>
-  </si>
-  <si>
-    <t>difficulty_offer4                              numeric</t>
-  </si>
-  <si>
-    <t>difficulty_offer5                              numeric</t>
-  </si>
-  <si>
-    <t>difficulty_offer6                              numeric</t>
-  </si>
-  <si>
-    <t>difficulty_offer7                              numeric</t>
-  </si>
-  <si>
-    <t>difficulty_offer8                              numeric</t>
-  </si>
-  <si>
-    <t>difficulty_offer9                              numeric</t>
-  </si>
-  <si>
-    <t>difficulty_offer10                             numeric</t>
-  </si>
-  <si>
-    <t>duration_offer1                                numeric</t>
-  </si>
-  <si>
-    <t>duration of award in hours one unique value</t>
-  </si>
-  <si>
-    <t>duration_offer2                                numeric</t>
-  </si>
-  <si>
-    <t>duration_offer3                                numeric</t>
-  </si>
-  <si>
-    <t>duration_offer4                                numeric</t>
-  </si>
-  <si>
-    <t>duration_offer5                                numeric</t>
-  </si>
-  <si>
-    <t>duration_offer6                                numeric</t>
-  </si>
-  <si>
-    <t>duration_offer7                                numeric</t>
-  </si>
-  <si>
-    <t>duration_offer8                                numeric</t>
-  </si>
-  <si>
-    <t>duration_offer9                                numeric</t>
-  </si>
-  <si>
-    <t>duration_offer10                               numeric</t>
-  </si>
-  <si>
-    <t>bogo_offer1                                    numeric</t>
-  </si>
-  <si>
-    <t>one unique value - is offer bogo</t>
-  </si>
-  <si>
-    <t>bogo_offer2                                    numeric</t>
-  </si>
-  <si>
-    <t>bogo_offer3                                    numeric</t>
-  </si>
-  <si>
-    <t>bogo_offer4                                    numeric</t>
-  </si>
-  <si>
-    <t>bogo_offer5                                    numeric</t>
-  </si>
-  <si>
-    <t>bogo_offer6                                    numeric</t>
-  </si>
-  <si>
-    <t>bogo_offer7                                    numeric</t>
-  </si>
-  <si>
-    <t>bogo_offer8                                    numeric</t>
-  </si>
-  <si>
-    <t>bogo_offer9                                    numeric</t>
-  </si>
-  <si>
-    <t>bogo_offer10                                   numeric</t>
-  </si>
-  <si>
-    <t>discount_offer1                                numeric</t>
-  </si>
-  <si>
-    <t>one unique value - is offer discount</t>
-  </si>
-  <si>
-    <t>discount_offer2                                numeric</t>
-  </si>
-  <si>
-    <t>discount_offer3                                numeric</t>
-  </si>
-  <si>
-    <t>discount_offer4                                numeric</t>
-  </si>
-  <si>
-    <t>discount_offer5                                numeric</t>
-  </si>
-  <si>
-    <t>discount_offer6                                numeric</t>
-  </si>
-  <si>
-    <t>discount_offer7                                numeric</t>
-  </si>
-  <si>
-    <t>discount_offer8                                numeric</t>
-  </si>
-  <si>
-    <t>discount_offer9                                numeric</t>
-  </si>
-  <si>
-    <t>discount_offer10                               numeric</t>
-  </si>
-  <si>
-    <t>informational_offer1                           numeric</t>
-  </si>
-  <si>
-    <t>one unique value - is offer informational</t>
-  </si>
-  <si>
-    <t>informational_offer2                           numeric</t>
-  </si>
-  <si>
-    <t>informational_offer3                           numeric</t>
-  </si>
-  <si>
-    <t>informational_offer4                           numeric</t>
-  </si>
-  <si>
-    <t>informational_offer5                           numeric</t>
-  </si>
-  <si>
-    <t>informational_offer6                           numeric</t>
-  </si>
-  <si>
-    <t>informational_offer7                           numeric</t>
-  </si>
-  <si>
-    <t>informational_offer8                           numeric</t>
-  </si>
-  <si>
-    <t>informational_offer9                           numeric</t>
-  </si>
-  <si>
-    <t>informational_offer10                          numeric</t>
-  </si>
-  <si>
-    <t>email_offer1                                   numeric</t>
-  </si>
-  <si>
-    <t>one unique value - is offer emailed</t>
-  </si>
-  <si>
-    <t>All offers are emailed - do we need? Also one unique value no variation to detect</t>
-  </si>
-  <si>
-    <t>email_offer2                                   numeric</t>
-  </si>
-  <si>
-    <t>email_offer3                                   numeric</t>
-  </si>
-  <si>
-    <t>email_offer4                                   numeric</t>
-  </si>
-  <si>
-    <t>email_offer5                                   numeric</t>
-  </si>
-  <si>
-    <t>email_offer6                                   numeric</t>
-  </si>
-  <si>
-    <t>email_offer7                                   numeric</t>
-  </si>
-  <si>
-    <t>email_offer8                                   numeric</t>
-  </si>
-  <si>
-    <t>email_offer9                                   numeric</t>
-  </si>
-  <si>
-    <t>email_offer10                                  numeric</t>
-  </si>
-  <si>
-    <t>mobile_offer1                                  numeric</t>
-  </si>
-  <si>
-    <t>one unique value - is offer mobile</t>
-  </si>
-  <si>
-    <t>Since all the same does it help in clustering?</t>
-  </si>
-  <si>
-    <t>mobile_offer2                                  numeric</t>
-  </si>
-  <si>
-    <t>mobile_offer3                                  numeric</t>
-  </si>
-  <si>
-    <t>mobile_offer4                                  numeric</t>
-  </si>
-  <si>
-    <t>mobile_offer5                                  numeric</t>
-  </si>
-  <si>
-    <t>mobile_offer6                                  numeric</t>
-  </si>
-  <si>
-    <t>mobile_offer7                                  numeric</t>
-  </si>
-  <si>
-    <t>mobile_offer8                                  numeric</t>
-  </si>
-  <si>
-    <t>mobile_offer9                                  numeric</t>
-  </si>
-  <si>
-    <t>mobile_offer10                                 numeric</t>
-  </si>
-  <si>
-    <t>social_offer1                                  numeric</t>
-  </si>
-  <si>
-    <t>social_offer2                                  numeric</t>
-  </si>
-  <si>
-    <t>social_offer3                                  numeric</t>
-  </si>
-  <si>
-    <t>social_offer4                                  numeric</t>
-  </si>
-  <si>
-    <t>social_offer5                                  numeric</t>
-  </si>
-  <si>
-    <t>social_offer6                                  numeric</t>
-  </si>
-  <si>
-    <t>social_offer7                                  numeric</t>
-  </si>
-  <si>
-    <t>social_offer8                                  numeric</t>
-  </si>
-  <si>
-    <t>social_offer9                                  numeric</t>
-  </si>
-  <si>
-    <t>social_offer10                                 numeric</t>
-  </si>
-  <si>
-    <t>web_offer1                                     numeric</t>
-  </si>
-  <si>
-    <t>one unique value - is offer web</t>
-  </si>
-  <si>
-    <t>web_offer2                                     numeric</t>
-  </si>
-  <si>
-    <t>web_offer3                                     numeric</t>
-  </si>
-  <si>
-    <t>web_offer4                                     numeric</t>
-  </si>
-  <si>
-    <t>web_offer5                                     numeric</t>
-  </si>
-  <si>
-    <t>web_offer6                                     numeric</t>
-  </si>
-  <si>
-    <t>web_offer7                                     numeric</t>
-  </si>
-  <si>
-    <t>web_offer8                                     numeric</t>
-  </si>
-  <si>
-    <t>web_offer9                                     numeric</t>
-  </si>
-  <si>
-    <t>web_offer10                                    numeric</t>
-  </si>
-  <si>
-    <t>offer_view_rate                                numeric</t>
-  </si>
-  <si>
-    <t>continuous between zero and one 5 nas</t>
-  </si>
-  <si>
-    <t>offer_completion_rate                          numeric</t>
-  </si>
-  <si>
-    <t>view_to_completion_rate                        numeric</t>
-  </si>
-  <si>
-    <t>continuous between zero and one - infinity and nan in</t>
-  </si>
-  <si>
-    <t>average_spend_per_transaction                  numeric</t>
-  </si>
-  <si>
-    <t>difference to ave_amount? 333 nas 0.15 to 451.47</t>
-  </si>
-  <si>
-    <t>spend_per_day                                  numeric</t>
-  </si>
-  <si>
     <t>membership date/tenure appears to be before transcript data starts</t>
   </si>
   <si>
@@ -780,6 +783,12 @@
     <t>0 to 5</t>
   </si>
   <si>
+    <t>perc_reward_cashed                             numeric</t>
+  </si>
+  <si>
+    <t>should be between 0 and 1 but some are above 1, inf appears due to total reward received=0</t>
+  </si>
+  <si>
     <t>RFM                                                                                                            factor</t>
   </si>
   <si>
@@ -805,13 +814,271 @@
   </si>
   <si>
     <t>M                                                                                                                    factor</t>
+  </si>
+  <si>
+    <t>New Variables</t>
+  </si>
+  <si>
+    <t>percentage of difficulty received</t>
+  </si>
+  <si>
+    <r>
+      <t>reward</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the monetary value of the promotion.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>channels</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the ways in which the promotion was advertised.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>difficulty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the amount the customer needs to spend in order to receive the reward.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>duration</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the total number of days that the promotion was available.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>offer_type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the type of promotion. This is either a money off offer (discount), buy one get one free (BOGO) or a news letter (informational).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the promotion identification.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>person</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the customer membership identification.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>event</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the event - either offer received, offer viewed, offer complete or transaction.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>value.offer.id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the promotion identification.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>value.amount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the amount spent in GBP for a given transaction.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>value.offer_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the promotion identification.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>value.reward</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the monetary value of the promotion.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> time from the beginning of the promotion period.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>gender</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the identified gender of the customer.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>age</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the age of the customer at the time of the promotion period.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the customer membership identification.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>became_member</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the date when the customer became a member.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>income</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF333333"/>
+        <rFont val="-Apple-System"/>
+        <charset val="1"/>
+      </rPr>
+      <t> is the self reported income of the customer at the time of the promotion period.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -833,6 +1100,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="-Apple-System"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="-Apple-System"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -891,13 +1171,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1212,17 +1495,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D197"/>
+  <dimension ref="A1:D226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C146" sqref="C146:C175"/>
+      <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A195" sqref="A195:XFD195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="64" style="2" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="67.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" style="2" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="2"/>
@@ -2933,9 +3216,6 @@
       <c r="B175" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C175" s="2" t="s">
-        <v>178</v>
-      </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" s="3" t="s">
@@ -2974,173 +3254,284 @@
         <v>216</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>14</v>
+        <v>217</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>14</v>
+        <v>217</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="3" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="194" spans="1:3">
-      <c r="A194" s="2" t="s">
-        <v>249</v>
+      <c r="A194" s="3" t="s">
+        <v>250</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C194" s="2" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="195" spans="1:3">
-      <c r="A195" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C195" s="2" t="s">
-        <v>254</v>
-      </c>
+      <c r="A195" s="3"/>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>256</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" ht="20.25">
+      <c r="A209" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" ht="42">
+      <c r="A210" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" ht="42">
+      <c r="A211" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" ht="42">
+      <c r="A212" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" ht="62.25">
+      <c r="A213" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" ht="20.25">
+      <c r="A214" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" ht="42">
+      <c r="A215" s="6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" ht="42">
+      <c r="A216" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" ht="20.25">
+      <c r="A217" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" ht="42">
+      <c r="A218" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" ht="20.25">
+      <c r="A219" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" ht="42">
+      <c r="A220" s="6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" ht="42">
+      <c r="A221" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" ht="20.25">
+      <c r="A222" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" ht="42">
+      <c r="A223" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" ht="20.25">
+      <c r="A224" s="6" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" ht="42">
+      <c r="A225" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" ht="42">
+      <c r="A226" s="6" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create dataframes of discount, bogo and informational
This removes people who don't get an award so need a full or right/left join to make sure no columns are missed
</commit_message>
<xml_diff>
--- a/wide format analysis.xlsx
+++ b/wide format analysis.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27417"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="241" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34882290-6755-4D01-BED6-E7A954CBBB34}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF8ACEB7-6BB9-4A80-8DA6-A1BBFF8717EA}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="283">
   <si>
     <t xml:space="preserve">Column Names                                                                                </t>
   </si>
@@ -786,7 +786,13 @@
     <t>perc_reward_cashed                             numeric</t>
   </si>
   <si>
-    <t>should be between 0 and 1 but some are above 1, inf appears due to total reward received=0</t>
+    <t>should be between 0 and 1 61 NAs no reward received</t>
+  </si>
+  <si>
+    <t>perc_difficulty_cashed                         numeric</t>
+  </si>
+  <si>
+    <t>should be between 0 and 1 61 no difficulty received</t>
   </si>
   <si>
     <t>RFM                                                                                                            factor</t>
@@ -1499,7 +1505,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A195" sqref="A195:XFD195"/>
+      <selection pane="bottomLeft" activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3394,144 +3400,149 @@
       </c>
     </row>
     <row r="195" spans="1:3">
-      <c r="A195" s="3"/>
+      <c r="A195" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="2" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="209" spans="1:1" ht="20.25">
       <c r="A209" s="6" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="210" spans="1:1" ht="42">
       <c r="A210" s="6" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="211" spans="1:1" ht="42">
       <c r="A211" s="6" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="212" spans="1:1" ht="42">
       <c r="A212" s="6" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="213" spans="1:1" ht="62.25">
       <c r="A213" s="6" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="214" spans="1:1" ht="20.25">
       <c r="A214" s="6" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="215" spans="1:1" ht="42">
       <c r="A215" s="6" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="216" spans="1:1" ht="42">
       <c r="A216" s="6" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="217" spans="1:1" ht="20.25">
       <c r="A217" s="6" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="218" spans="1:1" ht="42">
       <c r="A218" s="6" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="219" spans="1:1" ht="20.25">
       <c r="A219" s="6" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="220" spans="1:1" ht="42">
       <c r="A220" s="6" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="221" spans="1:1" ht="42">
       <c r="A221" s="6" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="222" spans="1:1" ht="20.25">
       <c r="A222" s="6" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="223" spans="1:1" ht="42">
       <c r="A223" s="6" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="224" spans="1:1" ht="20.25">
       <c r="A224" s="6" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="225" spans="1:1" ht="42">
       <c r="A225" s="6" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="226" spans="1:1" ht="42">
       <c r="A226" s="6" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding four new variables to speadsheet
</commit_message>
<xml_diff>
--- a/wide format analysis.xlsx
+++ b/wide format analysis.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="247" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF8ACEB7-6BB9-4A80-8DA6-A1BBFF8717EA}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22c422f4a98a0289/Documents/GitHub/DABI_project/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="270" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1C1239C-DF82-4463-9B57-C84CA127A242}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="291">
   <si>
     <t xml:space="preserve">Column Names                                                                                </t>
   </si>
@@ -1078,6 +1083,30 @@
       </rPr>
       <t> is the self reported income of the customer at the time of the promotion period.</t>
     </r>
+  </si>
+  <si>
+    <t>tot_tran_in                                    numeric</t>
+  </si>
+  <si>
+    <t>tot_amount_out                                 numeric</t>
+  </si>
+  <si>
+    <t>tot_amount_in                                  numeric</t>
+  </si>
+  <si>
+    <t>tot_tran_out                                   numeric</t>
+  </si>
+  <si>
+    <t>total transactions within offer periods</t>
+  </si>
+  <si>
+    <t>total transactions not within offer periods</t>
+  </si>
+  <si>
+    <t>total amount within offer periods</t>
+  </si>
+  <si>
+    <t>total amount not within offer periods</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1150,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1131,6 +1160,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1177,7 +1212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1187,6 +1222,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,9 +1242,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1245,7 +1282,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1351,7 +1388,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1493,7 +1530,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1501,20 +1538,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D226"/>
+  <dimension ref="A1:D230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B196" sqref="B196"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B180" sqref="B180"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="64" style="2" customWidth="1"/>
-    <col min="2" max="2" width="54.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="67.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="54.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="67.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1">
@@ -3224,324 +3261,360 @@
       </c>
     </row>
     <row r="176" spans="1:3">
-      <c r="A176" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>210</v>
-      </c>
+      <c r="A176" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C176" s="8"/>
     </row>
     <row r="177" spans="1:3">
-      <c r="A177" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>210</v>
-      </c>
+      <c r="A177" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C177" s="8"/>
     </row>
     <row r="178" spans="1:3">
-      <c r="A178" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>213</v>
-      </c>
+      <c r="A178" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="C178" s="8"/>
     </row>
     <row r="179" spans="1:3">
-      <c r="A179" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>215</v>
-      </c>
+      <c r="A179" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="C179" s="8"/>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="3" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C180" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="3" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C181" s="5" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="3" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="3" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C183" s="2" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="3" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>228</v>
+        <v>217</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="3" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>231</v>
+        <v>220</v>
+      </c>
+      <c r="C185" s="5" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="3" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="3" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="3" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C188" s="2" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="3" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>241</v>
+        <v>230</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="3" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>243</v>
+        <v>233</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="3" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>245</v>
+        <v>233</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="3" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>247</v>
+        <v>238</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="3" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B195" s="2" t="s">
+      <c r="B199" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
-      <c r="A196" s="2" t="s">
+    <row r="200" spans="1:3">
+      <c r="A200" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B196" s="2" t="s">
+      <c r="B200" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C196" s="2" t="s">
+      <c r="C200" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
-      <c r="A197" s="2" t="s">
+    <row r="201" spans="1:3">
+      <c r="A201" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B197" s="2" t="s">
+      <c r="B201" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C197" s="2" t="s">
+      <c r="C201" s="2" t="s">
         <v>259</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3">
-      <c r="A198" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3">
-      <c r="A199" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="204" spans="1:3">
-      <c r="A204" s="2" t="s">
+    <row r="208" spans="1:3">
+      <c r="A208" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="209" spans="1:1" ht="20.25">
-      <c r="A209" s="6" t="s">
+    <row r="213" spans="1:1" ht="17.399999999999999">
+      <c r="A213" s="6" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="210" spans="1:1" ht="42">
-      <c r="A210" s="6" t="s">
+    <row r="214" spans="1:1" ht="34.799999999999997">
+      <c r="A214" s="6" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="211" spans="1:1" ht="42">
-      <c r="A211" s="6" t="s">
+    <row r="215" spans="1:1" ht="34.799999999999997">
+      <c r="A215" s="6" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="212" spans="1:1" ht="42">
-      <c r="A212" s="6" t="s">
+    <row r="216" spans="1:1" ht="34.799999999999997">
+      <c r="A216" s="6" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="213" spans="1:1" ht="62.25">
-      <c r="A213" s="6" t="s">
+    <row r="217" spans="1:1" ht="52.2">
+      <c r="A217" s="6" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="214" spans="1:1" ht="20.25">
-      <c r="A214" s="6" t="s">
+    <row r="218" spans="1:1" ht="17.399999999999999">
+      <c r="A218" s="6" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="215" spans="1:1" ht="42">
-      <c r="A215" s="6" t="s">
+    <row r="219" spans="1:1" ht="17.399999999999999">
+      <c r="A219" s="6" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="216" spans="1:1" ht="42">
-      <c r="A216" s="6" t="s">
+    <row r="220" spans="1:1" ht="34.799999999999997">
+      <c r="A220" s="6" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="217" spans="1:1" ht="20.25">
-      <c r="A217" s="6" t="s">
+    <row r="221" spans="1:1" ht="17.399999999999999">
+      <c r="A221" s="6" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="218" spans="1:1" ht="42">
-      <c r="A218" s="6" t="s">
+    <row r="222" spans="1:1" ht="34.799999999999997">
+      <c r="A222" s="6" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="219" spans="1:1" ht="20.25">
-      <c r="A219" s="6" t="s">
+    <row r="223" spans="1:1" ht="17.399999999999999">
+      <c r="A223" s="6" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="220" spans="1:1" ht="42">
-      <c r="A220" s="6" t="s">
+    <row r="224" spans="1:1" ht="17.399999999999999">
+      <c r="A224" s="6" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="221" spans="1:1" ht="42">
-      <c r="A221" s="6" t="s">
+    <row r="225" spans="1:1" ht="17.399999999999999">
+      <c r="A225" s="6" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="222" spans="1:1" ht="20.25">
-      <c r="A222" s="6" t="s">
+    <row r="226" spans="1:1" ht="17.399999999999999">
+      <c r="A226" s="6" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="223" spans="1:1" ht="42">
-      <c r="A223" s="6" t="s">
+    <row r="227" spans="1:1" ht="34.799999999999997">
+      <c r="A227" s="6" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="224" spans="1:1" ht="20.25">
-      <c r="A224" s="6" t="s">
+    <row r="228" spans="1:1" ht="17.399999999999999">
+      <c r="A228" s="6" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="225" spans="1:1" ht="42">
-      <c r="A225" s="6" t="s">
+    <row r="229" spans="1:1" ht="34.799999999999997">
+      <c r="A229" s="6" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="226" spans="1:1" ht="42">
-      <c r="A226" s="6" t="s">
+    <row r="230" spans="1:1" ht="34.799999999999997">
+      <c r="A230" s="6" t="s">
         <v>282</v>
       </c>
     </row>

</xml_diff>

<commit_message>
create new sheet data_long
</commit_message>
<xml_diff>
--- a/wide format analysis.xlsx
+++ b/wide format analysis.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22c422f4a98a0289/Documents/GitHub/DABI_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="270" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1C1239C-DF82-4463-9B57-C84CA127A242}"/>
+  <xr:revisionPtr revIDLastSave="349" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB9FB5CD-CAB6-42B3-83E7-BEDCDE040C1C}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Wide" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Long" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="326">
   <si>
     <t xml:space="preserve">Column Names                                                                                </t>
   </si>
@@ -665,6 +666,30 @@
     <t>web_offer10                                    numeric</t>
   </si>
   <si>
+    <t>tot_tran_in                                    numeric</t>
+  </si>
+  <si>
+    <t>total transactions within offer periods</t>
+  </si>
+  <si>
+    <t>tot_tran_out                                   numeric</t>
+  </si>
+  <si>
+    <t>total transactions not within offer periods</t>
+  </si>
+  <si>
+    <t>tot_amount_in                                  numeric</t>
+  </si>
+  <si>
+    <t>total amount within offer periods</t>
+  </si>
+  <si>
+    <t>tot_amount_out                                 numeric</t>
+  </si>
+  <si>
+    <t>total amount not within offer periods</t>
+  </si>
+  <si>
     <t>offer_view_rate                                numeric</t>
   </si>
   <si>
@@ -800,7 +825,25 @@
     <t>should be between 0 and 1 61 no difficulty received</t>
   </si>
   <si>
-    <t>RFM                                                                                                            factor</t>
+    <t>r_score                                                                                                           int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 to 10 </t>
+  </si>
+  <si>
+    <t>does it add any insight</t>
+  </si>
+  <si>
+    <t>f_score                                                                                                            int</t>
+  </si>
+  <si>
+    <t>1 to 10</t>
+  </si>
+  <si>
+    <t>m_score                                                                                                          int</t>
+  </si>
+  <si>
+    <t>rfm_score                                                                                                     int</t>
   </si>
   <si>
     <t>3 to 30</t>
@@ -809,28 +852,16 @@
     <t>frequency and montary value are opposite direction so I believe it needs to be kept seperately</t>
   </si>
   <si>
-    <t>R                                                                                                                    Factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 to 10 </t>
-  </si>
-  <si>
-    <t>does it add any insight</t>
-  </si>
-  <si>
-    <t>F                                                                                                                     factor</t>
-  </si>
-  <si>
-    <t>1 to 10</t>
-  </si>
-  <si>
-    <t>M                                                                                                                    factor</t>
+    <t>rfm_string                                                                                                     int</t>
+  </si>
+  <si>
+    <t>111  to 101010</t>
   </si>
   <si>
     <t>New Variables</t>
   </si>
   <si>
-    <t>percentage of difficulty received</t>
+    <t>offers viewed by channel e.g. mobile, social and web</t>
   </si>
   <si>
     <r>
@@ -1085,28 +1116,103 @@
     </r>
   </si>
   <si>
-    <t>tot_tran_in                                    numeric</t>
-  </si>
-  <si>
-    <t>tot_amount_out                                 numeric</t>
-  </si>
-  <si>
-    <t>tot_amount_in                                  numeric</t>
-  </si>
-  <si>
-    <t>tot_tran_out                                   numeric</t>
-  </si>
-  <si>
-    <t>total transactions within offer periods</t>
-  </si>
-  <si>
-    <t>total transactions not within offer periods</t>
-  </si>
-  <si>
-    <t>total amount within offer periods</t>
-  </si>
-  <si>
-    <t>total amount not within offer periods</t>
+    <t>colnames(data_long)</t>
+  </si>
+  <si>
+    <t>person_id</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>70047 len</t>
+  </si>
+  <si>
+    <t>offer_num</t>
+  </si>
+  <si>
+    <t>transactions</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>0-36</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>0-1608</t>
+  </si>
+  <si>
+    <t>off_rec</t>
+  </si>
+  <si>
+    <t>0-6</t>
+  </si>
+  <si>
+    <t>off_view</t>
+  </si>
+  <si>
+    <t>off_comp</t>
+  </si>
+  <si>
+    <t>reward</t>
+  </si>
+  <si>
+    <t>0-50</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>membership_start</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>tenure</t>
+  </si>
+  <si>
+    <t>offer_id</t>
+  </si>
+  <si>
+    <t>reward_off</t>
+  </si>
+  <si>
+    <t>difficulty</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>bogo</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>informational</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>social</t>
+  </si>
+  <si>
+    <t>web</t>
   </si>
 </sst>
 </file>
@@ -1150,7 +1256,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1166,6 +1272,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1212,7 +1324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1224,6 +1336,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1242,9 +1358,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1282,7 +1398,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1388,7 +1504,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1530,7 +1646,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1538,20 +1654,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D230"/>
+  <dimension ref="A1:D231"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B180" sqref="B180"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="64" style="2" customWidth="1"/>
-    <col min="2" max="2" width="54.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="67.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="2"/>
+    <col min="2" max="2" width="54.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="67.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1">
@@ -3262,360 +3378,608 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176" s="7" t="s">
-        <v>283</v>
+        <v>209</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>287</v>
+        <v>210</v>
       </c>
       <c r="C176" s="8"/>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="7" t="s">
-        <v>286</v>
+        <v>211</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>288</v>
+        <v>212</v>
       </c>
       <c r="C177" s="8"/>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="7" t="s">
-        <v>285</v>
+        <v>213</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>289</v>
+        <v>214</v>
       </c>
       <c r="C178" s="8"/>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="7" t="s">
-        <v>284</v>
+        <v>215</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>290</v>
+        <v>216</v>
       </c>
       <c r="C179" s="8"/>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="3" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="3" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="3" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="3" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="3" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="3" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="3" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B187" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B187" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="C187" s="2" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="3" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="3" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="3" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="3" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="3" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="3" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="3" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="3" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="3" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="3" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3">
-      <c r="A198" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3">
-      <c r="A199" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3">
-      <c r="A200" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B200" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C200" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3">
-      <c r="A201" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B201" s="2" t="s">
+    </row>
+    <row r="198" spans="1:3" s="10" customFormat="1">
+      <c r="A198" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C201" s="2" t="s">
+      <c r="B198" s="10" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="202" spans="1:3">
-      <c r="A202" s="2" t="s">
+    <row r="199" spans="1:3" s="10" customFormat="1">
+      <c r="A199" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="B202" s="2" t="s">
+      <c r="B199" s="10" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
-      <c r="A203" s="2" t="s">
+    <row r="200" spans="1:3" s="10" customFormat="1">
+      <c r="A200" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="B203" s="2" t="s">
-        <v>261</v>
+      <c r="B200" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C200" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" s="10" customFormat="1">
+      <c r="A201" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="B201" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" s="10" customFormat="1">
+      <c r="A202" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="B202" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" s="10" customFormat="1">
+      <c r="A203" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B203" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="C203" s="10" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" s="10" customFormat="1">
+      <c r="A204" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B204" s="10" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3">
-      <c r="A208" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" ht="17.399999999999999">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" ht="17.45">
       <c r="A213" s="6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" ht="34.799999999999997">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" ht="34.9">
       <c r="A214" s="6" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="215" spans="1:1" ht="34.799999999999997">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" ht="34.9">
       <c r="A215" s="6" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" ht="34.799999999999997">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" ht="34.9">
       <c r="A216" s="6" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="217" spans="1:1" ht="52.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" ht="52.15">
       <c r="A217" s="6" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="218" spans="1:1" ht="17.399999999999999">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" ht="17.45">
       <c r="A218" s="6" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" ht="17.399999999999999">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" ht="17.45">
       <c r="A219" s="6" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="220" spans="1:1" ht="34.799999999999997">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" ht="34.9">
       <c r="A220" s="6" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" ht="17.399999999999999">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" ht="17.45">
       <c r="A221" s="6" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="222" spans="1:1" ht="34.799999999999997">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" ht="34.9">
       <c r="A222" s="6" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="223" spans="1:1" ht="17.399999999999999">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" ht="17.45">
       <c r="A223" s="6" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="224" spans="1:1" ht="17.399999999999999">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" ht="17.45">
       <c r="A224" s="6" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="225" spans="1:1" ht="17.399999999999999">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" ht="17.45">
       <c r="A225" s="6" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="226" spans="1:1" ht="17.399999999999999">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" ht="17.45">
       <c r="A226" s="6" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="227" spans="1:1" ht="34.799999999999997">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" ht="34.9">
       <c r="A227" s="6" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="228" spans="1:1" ht="17.399999999999999">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" ht="17.45">
       <c r="A228" s="6" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="229" spans="1:1" ht="34.799999999999997">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" ht="34.9">
       <c r="A229" s="6" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="230" spans="1:1" ht="34.799999999999997">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" ht="34.9">
       <c r="A230" s="6" t="s">
-        <v>282</v>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" ht="15"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1365EA1-BBC2-4E69-B838-29CB0BAA24EF}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="B4" t="s">
+        <v>299</v>
+      </c>
+      <c r="C4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="B6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="B7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="B8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="B9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C9" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="B10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="B11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="B12" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="B13" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="B14" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="B15" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="B16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="B17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="B18" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="B19" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="B20" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="B21" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="B22" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="B23" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="B24" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="B25" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>